<commit_message>
Updates xls for r2.
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-Picnic.xlsx
+++ b/heatmaps/R-scr/HM-Picnic.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="209">
   <si>
     <t>PgM</t>
   </si>
@@ -361,9 +361,6 @@
     <t>Helena Eberil</t>
   </si>
   <si>
-    <t>O6</t>
-  </si>
-  <si>
     <t>Simeon Soetan</t>
   </si>
   <si>
@@ -671,6 +668,15 @@
   </si>
   <si>
     <t>Dsgnr17</t>
+  </si>
+  <si>
+    <t>Anna Bergh</t>
+  </si>
+  <si>
+    <t>PjM2</t>
+  </si>
+  <si>
+    <t>PjM1</t>
   </si>
 </sst>
 </file>
@@ -1214,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1289,7 @@
         <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H3" t="s">
         <v>87</v>
@@ -1306,7 +1312,7 @@
         <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H4" t="s">
         <v>89</v>
@@ -1329,7 +1335,7 @@
         <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H5" t="s">
         <v>91</v>
@@ -1352,7 +1358,7 @@
         <v>92</v>
       </c>
       <c r="G6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H6" t="s">
         <v>93</v>
@@ -1421,7 +1427,7 @@
         <v>98</v>
       </c>
       <c r="G9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H9" t="s">
         <v>99</v>
@@ -1467,32 +1473,32 @@
         <v>102</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11" t="s">
-        <v>103</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H12" t="s">
         <v>104</v>
-      </c>
-      <c r="G12" t="s">
-        <v>174</v>
-      </c>
-      <c r="H12" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13" t="s">
         <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1500,7 +1506,7 @@
         <v>67</v>
       </c>
       <c r="G14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H14" t="s">
         <v>13</v>
@@ -1508,10 +1514,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" t="s">
         <v>109</v>
-      </c>
-      <c r="G15" t="s">
-        <v>110</v>
       </c>
       <c r="H15" t="s">
         <v>11</v>
@@ -1519,134 +1525,134 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" t="s">
         <v>111</v>
-      </c>
-      <c r="G16" t="s">
-        <v>179</v>
-      </c>
-      <c r="H16" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" t="s">
+        <v>173</v>
+      </c>
+      <c r="H17" t="s">
         <v>113</v>
-      </c>
-      <c r="G17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H17" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
+        <v>114</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" t="s">
         <v>115</v>
-      </c>
-      <c r="G18" t="s">
-        <v>110</v>
-      </c>
-      <c r="H18" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" t="s">
+        <v>161</v>
+      </c>
+      <c r="H19" t="s">
         <v>117</v>
-      </c>
-      <c r="G19" t="s">
-        <v>162</v>
-      </c>
-      <c r="H19" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" t="s">
+        <v>173</v>
+      </c>
+      <c r="H20" t="s">
         <v>119</v>
-      </c>
-      <c r="G20" t="s">
-        <v>174</v>
-      </c>
-      <c r="H20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" t="s">
+        <v>179</v>
+      </c>
+      <c r="H21" t="s">
         <v>121</v>
-      </c>
-      <c r="G21" t="s">
-        <v>180</v>
-      </c>
-      <c r="H21" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="22" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" t="s">
+        <v>180</v>
+      </c>
+      <c r="H22" t="s">
         <v>123</v>
-      </c>
-      <c r="G22" t="s">
-        <v>181</v>
-      </c>
-      <c r="H22" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="23" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H23" t="s">
         <v>125</v>
-      </c>
-      <c r="G23" t="s">
-        <v>181</v>
-      </c>
-      <c r="H23" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="24" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" t="s">
+        <v>181</v>
+      </c>
+      <c r="H24" t="s">
         <v>127</v>
-      </c>
-      <c r="G24" t="s">
-        <v>182</v>
-      </c>
-      <c r="H24" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="25" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" t="s">
+        <v>173</v>
+      </c>
+      <c r="H25" t="s">
         <v>129</v>
-      </c>
-      <c r="G25" t="s">
-        <v>174</v>
-      </c>
-      <c r="H25" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="26" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" t="s">
+        <v>173</v>
+      </c>
+      <c r="H26" t="s">
         <v>131</v>
-      </c>
-      <c r="G26" t="s">
-        <v>174</v>
-      </c>
-      <c r="H26" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="27" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
+        <v>132</v>
+      </c>
+      <c r="G27" t="s">
+        <v>173</v>
+      </c>
+      <c r="H27" t="s">
         <v>133</v>
-      </c>
-      <c r="G27" t="s">
-        <v>174</v>
-      </c>
-      <c r="H27" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="28" spans="6:8" x14ac:dyDescent="0.25">
@@ -1662,310 +1668,321 @@
     </row>
     <row r="29" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" t="s">
+        <v>182</v>
+      </c>
+      <c r="H29" t="s">
         <v>135</v>
-      </c>
-      <c r="G29" t="s">
-        <v>183</v>
-      </c>
-      <c r="H29" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="30" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" t="s">
         <v>137</v>
-      </c>
-      <c r="G30" t="s">
-        <v>110</v>
-      </c>
-      <c r="H30" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="31" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G31" t="s">
         <v>65</v>
       </c>
       <c r="H31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" t="s">
         <v>141</v>
-      </c>
-      <c r="G32" t="s">
-        <v>176</v>
-      </c>
-      <c r="H32" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" t="s">
+        <v>183</v>
+      </c>
+      <c r="H33" t="s">
         <v>143</v>
-      </c>
-      <c r="G33" t="s">
-        <v>184</v>
-      </c>
-      <c r="H33" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
+        <v>144</v>
+      </c>
+      <c r="G34" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" t="s">
         <v>145</v>
-      </c>
-      <c r="G34" t="s">
-        <v>110</v>
-      </c>
-      <c r="H34" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
+        <v>146</v>
+      </c>
+      <c r="G35" t="s">
+        <v>107</v>
+      </c>
+      <c r="H35" t="s">
         <v>147</v>
-      </c>
-      <c r="G35" t="s">
-        <v>108</v>
-      </c>
-      <c r="H35" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
+        <v>148</v>
+      </c>
+      <c r="G36" t="s">
+        <v>173</v>
+      </c>
+      <c r="H36" t="s">
         <v>149</v>
-      </c>
-      <c r="G36" t="s">
-        <v>174</v>
-      </c>
-      <c r="H36" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
+        <v>150</v>
+      </c>
+      <c r="G37" t="s">
+        <v>184</v>
+      </c>
+      <c r="H37" t="s">
         <v>151</v>
-      </c>
-      <c r="G37" t="s">
-        <v>185</v>
-      </c>
-      <c r="H37" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" t="s">
         <v>187</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>188</v>
-      </c>
-      <c r="H38" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
+        <v>189</v>
+      </c>
+      <c r="G39" t="s">
+        <v>183</v>
+      </c>
+      <c r="H39" t="s">
         <v>190</v>
-      </c>
-      <c r="G39" t="s">
-        <v>184</v>
-      </c>
-      <c r="H39" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
+        <v>191</v>
+      </c>
+      <c r="G40" t="s">
+        <v>183</v>
+      </c>
+      <c r="H40" t="s">
         <v>192</v>
-      </c>
-      <c r="G40" t="s">
-        <v>184</v>
-      </c>
-      <c r="H40" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="41" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
+        <v>195</v>
+      </c>
+      <c r="G43" t="s">
+        <v>183</v>
+      </c>
+      <c r="H43" t="s">
         <v>196</v>
-      </c>
-      <c r="G43" t="s">
-        <v>184</v>
-      </c>
-      <c r="H43" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="44" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
+        <v>197</v>
+      </c>
+      <c r="G44" t="s">
+        <v>183</v>
+      </c>
+      <c r="H44" t="s">
         <v>198</v>
-      </c>
-      <c r="G44" t="s">
-        <v>184</v>
-      </c>
-      <c r="H44" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="45" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
+        <v>199</v>
+      </c>
+      <c r="G45" t="s">
+        <v>180</v>
+      </c>
+      <c r="H45" t="s">
         <v>200</v>
-      </c>
-      <c r="G45" t="s">
-        <v>181</v>
-      </c>
-      <c r="H45" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="46" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
+        <v>201</v>
+      </c>
+      <c r="G46" t="s">
         <v>202</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>203</v>
-      </c>
-      <c r="H46" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="47" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G48" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
+        <v>158</v>
+      </c>
+      <c r="G50" t="s">
+        <v>185</v>
+      </c>
+      <c r="H50" t="s">
         <v>159</v>
-      </c>
-      <c r="G50" t="s">
-        <v>186</v>
-      </c>
-      <c r="H50" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="51" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
+        <v>160</v>
+      </c>
+      <c r="G51" t="s">
         <v>161</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>162</v>
-      </c>
-      <c r="H51" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="52" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
+        <v>163</v>
+      </c>
+      <c r="G52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H52" t="s">
         <v>164</v>
-      </c>
-      <c r="G52" t="s">
-        <v>162</v>
-      </c>
-      <c r="H52" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="53" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G53" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G54" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H55" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G56" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H56" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
         <v>206</v>
+      </c>
+      <c r="G57" t="s">
+        <v>84</v>
+      </c>
+      <c r="H57" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds r2 results for d4.
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-Picnic.xlsx
+++ b/heatmaps/R-scr/HM-Picnic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="216">
   <si>
     <t>PgM</t>
   </si>
@@ -683,6 +683,21 @@
   </si>
   <si>
     <t>Cirv2</t>
+  </si>
+  <si>
+    <t>Jonas Kullenwall</t>
+  </si>
+  <si>
+    <t>Dsngr18</t>
+  </si>
+  <si>
+    <t>Steffan Ehnebom</t>
+  </si>
+  <si>
+    <t>Senior Software Expert</t>
+  </si>
+  <si>
+    <t>SSE1</t>
   </si>
 </sst>
 </file>
@@ -1226,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2000,6 +2015,28 @@
       </c>
       <c r="H58" t="s">
         <v>210</v>
+      </c>
+    </row>
+    <row r="59" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>211</v>
+      </c>
+      <c r="G59" t="s">
+        <v>173</v>
+      </c>
+      <c r="H59" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>213</v>
+      </c>
+      <c r="G60" t="s">
+        <v>214</v>
+      </c>
+      <c r="H60" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds survey response for d5 (r2)
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-Picnic.xlsx
+++ b/heatmaps/R-scr/HM-Picnic.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="230">
   <si>
     <t>PgM</t>
   </si>
@@ -698,6 +698,48 @@
   </si>
   <si>
     <t>SSE1</t>
+  </si>
+  <si>
+    <t>Carl Waite</t>
+  </si>
+  <si>
+    <t>System Verification</t>
+  </si>
+  <si>
+    <t>SV1</t>
+  </si>
+  <si>
+    <t>Henrik Eriksson H</t>
+  </si>
+  <si>
+    <t>Functional Verification Eng</t>
+  </si>
+  <si>
+    <t>FVE1</t>
+  </si>
+  <si>
+    <t>Peter Bjurenhäll</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Dsgnr19</t>
+  </si>
+  <si>
+    <t>Henrik Schreiber</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>LM1</t>
+  </si>
+  <si>
+    <t>Ann Jeanette Jatko</t>
+  </si>
+  <si>
+    <t>Dsgnr20</t>
   </si>
 </sst>
 </file>
@@ -1241,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2037,6 +2079,61 @@
       </c>
       <c r="H60" t="s">
         <v>215</v>
+      </c>
+    </row>
+    <row r="61" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>216</v>
+      </c>
+      <c r="G61" t="s">
+        <v>217</v>
+      </c>
+      <c r="H61" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="62" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>219</v>
+      </c>
+      <c r="G62" t="s">
+        <v>220</v>
+      </c>
+      <c r="H62" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="63" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>222</v>
+      </c>
+      <c r="G63" t="s">
+        <v>223</v>
+      </c>
+      <c r="H63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="64" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>225</v>
+      </c>
+      <c r="G64" t="s">
+        <v>226</v>
+      </c>
+      <c r="H64" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="65" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>228</v>
+      </c>
+      <c r="G65" t="s">
+        <v>173</v>
+      </c>
+      <c r="H65" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>